<commit_message>
Rename CNN.m to main.m
</commit_message>
<xml_diff>
--- a/confusion_matrix.xlsx
+++ b/confusion_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pennstateoffice365-my.sharepoint.com/personal/bbm5449_psu_edu/Documents/2023 Fall/CMPEN 454/Project1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6DDE7126-B60C-4696-B37B-AF7F08F284F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="8_{6DDE7126-B60C-4696-B37B-AF7F08F284F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF15191B-E378-4DDB-B335-C51725A0F45D}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6636759B-0D2B-42A8-B1A8-06A3B7BD901E}"/>
   </bookViews>
@@ -385,10 +385,13 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.7265625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1">

</xml_diff>

<commit_message>
Upload video and slides
</commit_message>
<xml_diff>
--- a/confusion_matrix.xlsx
+++ b/confusion_matrix.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pennstateoffice365-my.sharepoint.com/personal/bbm5449_psu_edu/Documents/2023 Fall/CMPEN 454/Project1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{6DDE7126-B60C-4696-B37B-AF7F08F284F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF15191B-E378-4DDB-B335-C51725A0F45D}"/>
+  <xr:revisionPtr revIDLastSave="93" documentId="8_{6DDE7126-B60C-4696-B37B-AF7F08F284F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CAB82DEB-547A-4B3F-A9D7-86D082299CD5}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6636759B-0D2B-42A8-B1A8-06A3B7BD901E}"/>
   </bookViews>
@@ -35,9 +35,44 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="10">
+  <si>
+    <t>'airplane'</t>
+  </si>
+  <si>
+    <t>'automobile'</t>
+  </si>
+  <si>
+    <t>'bird'</t>
+  </si>
+  <si>
+    <t>'cat'</t>
+  </si>
+  <si>
+    <t>'deer'</t>
+  </si>
+  <si>
+    <t>'dog'</t>
+  </si>
+  <si>
+    <t>'frog'</t>
+  </si>
+  <si>
+    <t>'horse'</t>
+  </si>
+  <si>
+    <t>'ship'</t>
+  </si>
+  <si>
+    <t>'truck'</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -45,16 +80,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -62,18 +111,47 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF3300"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -83,6 +161,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -382,335 +464,484 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD2E3B06-8074-4A98-88B5-3D4EECC4B94C}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:P53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.7265625" customWidth="1"/>
+    <col min="4" max="5" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A1" s="2"/>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
         <v>531</v>
       </c>
-      <c r="B1">
+      <c r="C2" s="3">
         <v>41</v>
       </c>
-      <c r="C1">
+      <c r="D2" s="3">
         <v>65</v>
       </c>
-      <c r="D1">
+      <c r="E2" s="3">
         <v>37</v>
       </c>
-      <c r="E1">
+      <c r="F2" s="3">
         <v>10</v>
       </c>
-      <c r="F1">
+      <c r="G2" s="3">
         <v>8</v>
       </c>
-      <c r="G1">
+      <c r="H2" s="3">
         <v>18</v>
       </c>
-      <c r="H1">
+      <c r="I2" s="3">
         <v>38</v>
       </c>
-      <c r="I1">
+      <c r="J2" s="3">
         <v>210</v>
       </c>
-      <c r="J1">
+      <c r="K2" s="3">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3">
         <v>40</v>
       </c>
-      <c r="B2">
+      <c r="C3" s="1">
         <v>519</v>
       </c>
-      <c r="C2">
+      <c r="D3" s="3">
         <v>9</v>
       </c>
-      <c r="D2">
+      <c r="E3" s="3">
         <v>26</v>
       </c>
-      <c r="E2">
+      <c r="F3" s="3">
         <v>10</v>
       </c>
-      <c r="F2">
+      <c r="G3" s="3">
         <v>7</v>
       </c>
-      <c r="G2">
+      <c r="H3" s="3">
         <v>19</v>
       </c>
-      <c r="H2">
+      <c r="I3" s="3">
         <v>29</v>
       </c>
-      <c r="I2">
+      <c r="J3" s="3">
         <v>111</v>
       </c>
-      <c r="J2">
+      <c r="K3" s="3">
         <v>230</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
         <v>87</v>
       </c>
-      <c r="B3">
+      <c r="C4" s="3">
         <v>8</v>
       </c>
-      <c r="C3">
+      <c r="D4" s="1">
         <v>386</v>
       </c>
-      <c r="D3">
+      <c r="E4" s="3">
         <v>117</v>
       </c>
-      <c r="E3">
+      <c r="F4" s="3">
         <v>97</v>
       </c>
-      <c r="F3">
+      <c r="G4" s="3">
         <v>70</v>
       </c>
-      <c r="G3">
+      <c r="H4" s="3">
         <v>104</v>
       </c>
-      <c r="H3">
+      <c r="I4" s="3">
         <v>88</v>
       </c>
-      <c r="I3">
+      <c r="J4" s="3">
         <v>25</v>
       </c>
-      <c r="J3">
+      <c r="K4" s="3">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3">
         <v>39</v>
       </c>
-      <c r="B4">
+      <c r="C5" s="3">
         <v>18</v>
       </c>
-      <c r="C4">
+      <c r="D5" s="3">
         <v>127</v>
       </c>
-      <c r="D4">
+      <c r="E5" s="1">
         <v>325</v>
       </c>
-      <c r="E4">
+      <c r="F5" s="3">
         <v>45</v>
       </c>
-      <c r="F4">
+      <c r="G5" s="3">
         <v>136</v>
       </c>
-      <c r="G4">
+      <c r="H5" s="3">
         <v>186</v>
       </c>
-      <c r="H4">
+      <c r="I5" s="3">
         <v>89</v>
       </c>
-      <c r="I4">
+      <c r="J5" s="3">
         <v>13</v>
       </c>
-      <c r="J4">
+      <c r="K5" s="3">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3">
         <v>53</v>
       </c>
-      <c r="B5">
+      <c r="C6" s="3">
         <v>6</v>
       </c>
-      <c r="C5">
+      <c r="D6" s="3">
         <v>270</v>
       </c>
-      <c r="D5">
+      <c r="E6" s="3">
         <v>69</v>
       </c>
-      <c r="E5">
+      <c r="F6" s="1">
         <v>259</v>
       </c>
-      <c r="F5">
+      <c r="G6" s="3">
         <v>38</v>
       </c>
-      <c r="G5">
+      <c r="H6" s="3">
         <v>162</v>
       </c>
-      <c r="H5">
+      <c r="I6" s="3">
         <v>114</v>
       </c>
-      <c r="I5">
+      <c r="J6" s="3">
         <v>22</v>
       </c>
-      <c r="J5">
+      <c r="K6" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3">
         <v>19</v>
       </c>
-      <c r="B6">
+      <c r="C7" s="3">
         <v>7</v>
       </c>
-      <c r="C6">
+      <c r="D7" s="3">
         <v>151</v>
       </c>
-      <c r="D6">
+      <c r="E7" s="3">
         <v>222</v>
       </c>
-      <c r="E6">
+      <c r="F7" s="3">
         <v>49</v>
       </c>
-      <c r="F6">
+      <c r="G7" s="1">
         <v>281</v>
       </c>
-      <c r="G6">
+      <c r="H7" s="3">
         <v>111</v>
       </c>
-      <c r="H6">
+      <c r="I7" s="3">
         <v>125</v>
       </c>
-      <c r="I6">
+      <c r="J7" s="3">
         <v>20</v>
       </c>
-      <c r="J6">
+      <c r="K7" s="3">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3">
         <v>10</v>
       </c>
-      <c r="B7">
+      <c r="C8" s="3">
         <v>7</v>
       </c>
-      <c r="C7">
+      <c r="D8" s="3">
         <v>120</v>
       </c>
-      <c r="D7">
+      <c r="E8" s="3">
         <v>125</v>
       </c>
-      <c r="E7">
+      <c r="F8" s="3">
         <v>93</v>
       </c>
-      <c r="F7">
+      <c r="G8" s="3">
         <v>23</v>
       </c>
-      <c r="G7">
+      <c r="H8" s="1">
         <v>557</v>
       </c>
-      <c r="H7">
+      <c r="I8" s="3">
         <v>33</v>
       </c>
-      <c r="I7">
+      <c r="J8" s="3">
         <v>9</v>
       </c>
-      <c r="J7">
+      <c r="K8" s="3">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3">
         <v>32</v>
       </c>
-      <c r="B8">
+      <c r="C9" s="3">
         <v>7</v>
       </c>
-      <c r="C8">
+      <c r="D9" s="3">
         <v>73</v>
       </c>
-      <c r="D8">
+      <c r="E9" s="3">
         <v>98</v>
       </c>
-      <c r="E8">
+      <c r="F9" s="3">
         <v>77</v>
       </c>
-      <c r="F8">
+      <c r="G9" s="3">
         <v>94</v>
       </c>
-      <c r="G8">
+      <c r="H9" s="3">
         <v>54</v>
       </c>
-      <c r="H8">
+      <c r="I9" s="1">
         <v>533</v>
       </c>
-      <c r="I8">
+      <c r="J9" s="3">
         <v>13</v>
       </c>
-      <c r="J8">
+      <c r="K9" s="3">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3">
         <v>192</v>
       </c>
-      <c r="B9">
+      <c r="C10" s="3">
         <v>84</v>
       </c>
-      <c r="C9">
+      <c r="D10" s="3">
         <v>35</v>
       </c>
-      <c r="D9">
+      <c r="E10" s="3">
         <v>44</v>
       </c>
-      <c r="E9">
+      <c r="F10" s="3">
         <v>7</v>
       </c>
-      <c r="F9">
+      <c r="G10" s="3">
         <v>8</v>
       </c>
-      <c r="G9">
+      <c r="H10" s="3">
         <v>10</v>
       </c>
-      <c r="H9">
+      <c r="I10" s="3">
         <v>16</v>
       </c>
-      <c r="I9">
+      <c r="J10" s="1">
         <v>542</v>
       </c>
-      <c r="J9">
+      <c r="K10" s="3">
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3">
         <v>69</v>
       </c>
-      <c r="B10">
+      <c r="C11" s="3">
         <v>191</v>
       </c>
-      <c r="C10">
+      <c r="D11" s="3">
         <v>23</v>
       </c>
-      <c r="D10">
+      <c r="E11" s="3">
         <v>41</v>
       </c>
-      <c r="E10">
+      <c r="F11" s="3">
         <v>4</v>
       </c>
-      <c r="F10">
+      <c r="G11" s="3">
         <v>9</v>
       </c>
-      <c r="G10">
+      <c r="H11" s="3">
         <v>30</v>
       </c>
-      <c r="H10">
+      <c r="I11" s="3">
         <v>68</v>
       </c>
-      <c r="I10">
+      <c r="J11" s="3">
         <v>127</v>
       </c>
-      <c r="J10">
+      <c r="K11" s="1">
         <v>438</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P12" s="4"/>
+    </row>
+    <row r="23" spans="6:15" x14ac:dyDescent="0.35">
+      <c r="F23" t="s">
+        <v>0</v>
+      </c>
+      <c r="G23" t="s">
+        <v>1</v>
+      </c>
+      <c r="H23" t="s">
+        <v>2</v>
+      </c>
+      <c r="I23" t="s">
+        <v>3</v>
+      </c>
+      <c r="J23" t="s">
+        <v>4</v>
+      </c>
+      <c r="K23" t="s">
+        <v>5</v>
+      </c>
+      <c r="L23" t="s">
+        <v>6</v>
+      </c>
+      <c r="M23" t="s">
+        <v>7</v>
+      </c>
+      <c r="N23" t="s">
+        <v>8</v>
+      </c>
+      <c r="O23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F44" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F45" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F46" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F47" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F48" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F49" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F50" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F51" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F52" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F53" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>